<commit_message>
laid out most of the analysis
</commit_message>
<xml_diff>
--- a/ss_order.xlsx
+++ b/ss_order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgarber\Jup\PhD_jup\GIS_scripts_dendro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A169888F-9EF0-4D82-9879-1AD61211F10E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4776CC00-697C-47EE-95C7-4CF9471BF232}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D0264D5F-37E4-416F-B5E8-AEFA1A8EDD51}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>silt</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>fine gravel</t>
+  </si>
+  <si>
+    <t>loam</t>
   </si>
 </sst>
 </file>
@@ -458,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC7FE9BD-7B4A-44D5-AF50-38708306CABD}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +504,7 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -510,7 +513,7 @@
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -519,7 +522,7 @@
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -528,7 +531,7 @@
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -537,7 +540,7 @@
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -546,7 +549,7 @@
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -555,7 +558,7 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -564,7 +567,7 @@
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -573,7 +576,7 @@
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>11</v>
@@ -581,7 +584,12 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
@@ -630,6 +638,10 @@
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>